<commit_message>
update 8 _ check url public
</commit_message>
<xml_diff>
--- a/ttcn2_ETest-master/src/main/java/com/example/ttcn2etest/upload/loi_nhap_du_lieu.xlsx
+++ b/ttcn2_ETest-master/src/main/java/com/example/ttcn2etest/upload/loi_nhap_du_lieu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Họ và tên</t>
   </si>
@@ -41,19 +41,19 @@
     <t>0833333333</t>
   </si>
   <si>
-    <t>nguyenthiAb1@gmail.com</t>
+    <t>lienltw25@gmail.com</t>
+  </si>
+  <si>
+    <t>17/02/2002</t>
   </si>
   <si>
     <t>Phù Chẩn - Từ Sơn -Bắc Ninh</t>
   </si>
   <si>
-    <t>kjhgfds11</t>
-  </si>
-  <si>
-    <t>Email already exists</t>
-  </si>
-  <si>
-    <t>Username already exists</t>
+    <t>lienltw25</t>
+  </si>
+  <si>
+    <t>Username đã tồn tại trong hệ thống!</t>
   </si>
   <si>
     <t>Dương Thanh Lâm</t>
@@ -62,37 +62,64 @@
     <t>0943333333</t>
   </si>
   <si>
-    <t>nguyenthib11@gmail.com</t>
-  </si>
-  <si>
-    <t>jhgfdsahg21</t>
+    <t>lienltwAD@gmail.com</t>
+  </si>
+  <si>
+    <t>17/02/2003</t>
+  </si>
+  <si>
+    <t>lienltwADMIN</t>
   </si>
   <si>
     <t>Nguyễn Văn Dương</t>
   </si>
   <si>
-    <t>nguyenthiC34@gmail.com</t>
-  </si>
-  <si>
-    <t>ytrewe31</t>
+    <t>phuongmai12@gmail.com</t>
+  </si>
+  <si>
+    <t>17/02/2004</t>
+  </si>
+  <si>
+    <t>phuongmai</t>
   </si>
   <si>
     <t>Đặng Vũ Hùng</t>
   </si>
   <si>
-    <t>nguyenthiD52@gmail.com</t>
-  </si>
-  <si>
-    <t>jhgffd41</t>
+    <t>kimlan0202@gmail.com</t>
+  </si>
+  <si>
+    <t>17/02/2005</t>
+  </si>
+  <si>
+    <t>kimlan02</t>
   </si>
   <si>
     <t>Nguyễn Tiến Sơn</t>
   </si>
   <si>
-    <t>nguyenthiE64@gmail.com</t>
-  </si>
-  <si>
-    <t>mnbvcx51</t>
+    <t>tangnguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>17/02/2006</t>
+  </si>
+  <si>
+    <t>tangnguyen</t>
+  </si>
+  <si>
+    <t>tangnguyenvan</t>
+  </si>
+  <si>
+    <t>thunguyen24@gmail.com</t>
+  </si>
+  <si>
+    <t>thunguyen</t>
+  </si>
+  <si>
+    <t>kimmai@gmail.com</t>
+  </si>
+  <si>
+    <t>lienltw34</t>
   </si>
 </sst>
 </file>
@@ -148,7 +175,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -184,14 +211,14 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>37304.0</v>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -207,37 +234,37 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n">
-        <v>37669.0</v>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" t="s" s="1">
-        <v>13</v>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="D4" t="n">
-        <v>38034.0</v>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -248,48 +275,117 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="D5" t="n">
-        <v>38400.0</v>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="G5" t="s" s="1">
-        <v>13</v>
+      <c r="G5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s" s="1">
-        <v>12</v>
-      </c>
-      <c r="D6" t="n">
-        <v>38765.0</v>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="G6" t="s" s="1">
-        <v>13</v>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>